<commit_message>
Adding files saved before quitting
	modified:   _LPN/LPN Draft Description.docx
	modified:   _RFR/RFR Draft Description.docx
	modified:   _SMC/SMC Class Transitions.xlsx
</commit_message>
<xml_diff>
--- a/_SMC/SMC Class Transitions.xlsx
+++ b/_SMC/SMC Class Transitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="0" windowWidth="20320" windowHeight="21220" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="2740" yWindow="0" windowWidth="19460" windowHeight="15480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mesic" sheetId="1" r:id="rId1"/>
@@ -629,8 +629,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -770,18 +776,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -800,8 +794,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -847,6 +853,9 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -892,6 +901,9 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1223,9 +1235,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2581,10 +2593,10 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="28">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="37" t="s">
         <v>73</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -2598,10 +2610,10 @@
       <c r="G2" s="15">
         <v>16</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="33" t="s">
         <v>65</v>
       </c>
       <c r="L2" s="15" t="s">
@@ -2617,8 +2629,8 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="28">
-      <c r="A3" s="34"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="15" t="s">
         <v>67</v>
       </c>
@@ -2630,8 +2642,8 @@
       <c r="G3" s="15">
         <v>84</v>
       </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="38"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="34"/>
       <c r="L3" s="15" t="s">
         <v>67</v>
       </c>
@@ -2645,8 +2657,8 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" thickBot="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="16" t="s">
         <v>51</v>
       </c>
@@ -2660,8 +2672,8 @@
         <v>80</v>
       </c>
       <c r="G4" s="16"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="38"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="34"/>
       <c r="L4" s="16" t="s">
         <v>51</v>
       </c>
@@ -2677,8 +2689,8 @@
       <c r="P4" s="16"/>
     </row>
     <row r="5" spans="1:16" ht="28">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37" t="s">
         <v>74</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -2688,8 +2700,8 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="38" t="s">
+      <c r="J5" s="32"/>
+      <c r="K5" s="34" t="s">
         <v>68</v>
       </c>
       <c r="L5" s="15" t="s">
@@ -2705,8 +2717,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="28">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="15" t="s">
         <v>67</v>
       </c>
@@ -2714,8 +2726,8 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="38"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="34"/>
       <c r="L6" s="15" t="s">
         <v>67</v>
       </c>
@@ -2729,8 +2741,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="16" thickBot="1">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="16" t="s">
         <v>51</v>
       </c>
@@ -2738,8 +2750,8 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="39"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="35"/>
       <c r="L7" s="16" t="s">
         <v>51</v>
       </c>
@@ -2755,8 +2767,8 @@
       <c r="P7" s="16"/>
     </row>
     <row r="8" spans="1:16" ht="28">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="37"/>
+      <c r="B8" s="37" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -2766,10 +2778,10 @@
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
-      <c r="J8" s="36" t="s">
+      <c r="J8" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="33" t="s">
         <v>65</v>
       </c>
       <c r="L8" s="15" t="s">
@@ -2781,8 +2793,8 @@
       <c r="P8" s="15"/>
     </row>
     <row r="9" spans="1:16" ht="28">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="15" t="s">
         <v>67</v>
       </c>
@@ -2790,8 +2802,8 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="38"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="34"/>
       <c r="L9" s="15" t="s">
         <v>67</v>
       </c>
@@ -2801,8 +2813,8 @@
       <c r="P9" s="15"/>
     </row>
     <row r="10" spans="1:16" ht="16" thickBot="1">
-      <c r="A10" s="34"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="16" t="s">
         <v>51</v>
       </c>
@@ -2810,8 +2822,8 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="39"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="35"/>
       <c r="L10" s="16" t="s">
         <v>51</v>
       </c>
@@ -2821,10 +2833,10 @@
       <c r="P10" s="16"/>
     </row>
     <row r="11" spans="1:16" ht="28">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="37" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -2836,8 +2848,8 @@
       <c r="G11" s="17"/>
     </row>
     <row r="12" spans="1:16" ht="28">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="15" t="s">
         <v>67</v>
       </c>
@@ -2847,8 +2859,8 @@
       <c r="G12" s="17"/>
     </row>
     <row r="13" spans="1:16" ht="16" thickBot="1">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="16" t="s">
         <v>51</v>
       </c>
@@ -2859,7 +2871,7 @@
     </row>
     <row r="16" spans="1:16" ht="16" thickBot="1"/>
     <row r="17" spans="1:6" ht="28">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="38" t="s">
         <v>76</v>
       </c>
       <c r="B17" s="18" t="s">
@@ -2879,7 +2891,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29" thickBot="1">
-      <c r="A18" s="33"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="16" t="s">
         <v>78</v>
       </c>
@@ -2897,41 +2909,41 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="38" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="31"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" ht="16" thickBot="1">
-      <c r="A20" s="33"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="38" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="15" t="s">
@@ -2945,9 +2957,9 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
       <c r="D22" s="15" t="s">
         <v>88</v>
       </c>
@@ -2959,9 +2971,9 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" thickBot="1">
-      <c r="A23" s="33"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="16" t="s">
         <v>84</v>
       </c>
@@ -2973,13 +2985,13 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="38" t="s">
         <v>85</v>
       </c>
       <c r="D24" s="15" t="s">
@@ -2988,30 +3000,30 @@
       <c r="E24" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="38" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16" thickBot="1">
-      <c r="A25" s="33"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="33"/>
+      <c r="F25" s="39"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="38" t="s">
         <v>85</v>
       </c>
       <c r="D26" s="15" t="s">
@@ -3020,30 +3032,30 @@
       <c r="E26" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="38" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16" thickBot="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
       <c r="D27" s="16" t="s">
         <v>84</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="33"/>
+      <c r="F27" s="39"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="38" t="s">
         <v>85</v>
       </c>
       <c r="D28" s="15" t="s">
@@ -3057,9 +3069,9 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
       <c r="D29" s="15" t="s">
         <v>88</v>
       </c>
@@ -3071,9 +3083,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="16" thickBot="1">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="16" t="s">
         <v>84</v>
       </c>
@@ -3101,18 +3113,17 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="J2:J7"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="K8:K10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="F26:F27"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
@@ -3121,17 +3132,18 @@
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="J2:J7"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="K8:K10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8612,7 +8624,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>